<commit_message>
6-8-2018 Completed the organic matter model, documentation, API, and test scripts. Minor modifications to the nutrients and volume model so that instantiation is possible without model execution. Updated the programmer's test log and added all relevant test JSONS to the OrganicMatter/TEST directory. Wrote code to thoroughly check data requirements for the AQUATOX organic matter model. Added to the documentation information about data requirements and potential links from other models within the JSON input.
</commit_message>
<xml_diff>
--- a/Data.Simulate.AQUATOX/DOCS/HMS_AQUATOX_Models_and_Requirements.xlsx
+++ b/Data.Simulate.AQUATOX/DOCS/HMS_AQUATOX_Models_and_Requirements.xlsx
@@ -86,9 +86,6 @@
     <t>Organic Matter, soft requirement.</t>
   </si>
   <si>
-    <t>TBA</t>
-  </si>
-  <si>
     <t>Animals and Plants, soft requirement</t>
   </si>
   <si>
@@ -125,13 +122,16 @@
     <t>Oxygen model or Driving Var.</t>
   </si>
   <si>
-    <t>Erosion / depositin rates, soft requirement</t>
-  </si>
-  <si>
     <t>AQTNutrientsModel.CheckDataRequirements</t>
   </si>
   <si>
     <t>Dissolved Org Matter or Driving Vars., soft</t>
+  </si>
+  <si>
+    <t>AQTOrganicMatter.CheckDataRequirements</t>
+  </si>
+  <si>
+    <t>Erosion / deposition rates, soft requirement</t>
   </si>
 </sst>
 </file>
@@ -596,7 +596,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,10 +738,10 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -749,10 +749,10 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3"/>
     </row>
@@ -784,7 +784,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -792,10 +792,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -803,7 +803,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="3"/>
     </row>
@@ -812,7 +812,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="3"/>
     </row>
@@ -830,134 +830,134 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor refinements to XML output.
</commit_message>
<xml_diff>
--- a/Data.Simulate.AQUATOX/DOCS/HMS_AQUATOX_Models_and_Requirements.xlsx
+++ b/Data.Simulate.AQUATOX/DOCS/HMS_AQUATOX_Models_and_Requirements.xlsx
@@ -44,9 +44,6 @@
     <t>Valid JSON with type bindings</t>
   </si>
   <si>
-    <t>Non-Zero State Variables in Simulation</t>
-  </si>
-  <si>
     <t>Valid PSETUP inputs</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>Erosion / deposition rates, soft requirement</t>
+  </si>
+  <si>
+    <t>One or more State Variables in Simulation</t>
   </si>
 </sst>
 </file>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
@@ -606,7 +606,7 @@
     <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +614,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -633,10 +633,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -644,10 +644,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,10 +669,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -680,10 +680,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,10 +691,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,74 +702,74 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3"/>
     </row>
@@ -778,50 +778,50 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,134 +830,134 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
         <v>31</v>
       </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed HMS Chemical Fate Model. Completed documentation for HMS Chemical Fate Model. Set up the test scripts and "Check Data Requirements" for the HMS Chemical Fate model. Added tests to check data requirements within JSON for chemical model. Ran all tests successfully. Refined CheckDataRequirements for nutrients model. Re-ran all AQUATOX test scripts successfully
</commit_message>
<xml_diff>
--- a/Data.Simulate.AQUATOX/DOCS/HMS_AQUATOX_Models_and_Requirements.xlsx
+++ b/Data.Simulate.AQUATOX/DOCS/HMS_AQUATOX_Models_and_Requirements.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="51">
   <si>
     <t>Model</t>
   </si>
@@ -132,6 +132,42 @@
   </si>
   <si>
     <t>One or more State Variables in Simulation</t>
+  </si>
+  <si>
+    <t>Chemical Fate Model</t>
+  </si>
+  <si>
+    <t>Diagenesis Model</t>
+  </si>
+  <si>
+    <t>Water Column Nutrients</t>
+  </si>
+  <si>
+    <t>AQTDiagenesisModel.CheckDataRequirements</t>
+  </si>
+  <si>
+    <t>POC, PON, POP state variables G1 to G3</t>
+  </si>
+  <si>
+    <t>Phosphate Ammonia Nitrate L1 and L2</t>
+  </si>
+  <si>
+    <t>Detritivores eating sediment bed (soft)</t>
+  </si>
+  <si>
+    <t>Animals Plants, OM depositing to sediment bed (soft requirement)</t>
+  </si>
+  <si>
+    <t>AQTChemicalModel.CheckDataRequirements</t>
+  </si>
+  <si>
+    <t>Light loadings</t>
+  </si>
+  <si>
+    <t>Animals Plants, OM sorption and desorption (soft requirement)</t>
+  </si>
+  <si>
+    <t>Chemical in water column state var (TToxics)</t>
   </si>
 </sst>
 </file>
@@ -162,12 +198,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,12 +224,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,7 +604,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,28 +636,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
     <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -749,70 +793,72 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C22" s="3"/>
     </row>
@@ -821,30 +867,28 @@
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-    </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>34</v>
@@ -855,29 +899,29 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="C28" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -885,38 +929,38 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="C32" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="C33" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>36</v>
@@ -927,7 +971,7 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>36</v>
@@ -938,18 +982,21 @@
         <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>22</v>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -957,7 +1004,173 @@
         <v>30</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>